<commit_message>
Atualização automática de RIO_GRANDE.xlsx
</commit_message>
<xml_diff>
--- a/RIO_GRANDE.xlsx
+++ b/RIO_GRANDE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F9775C7-12C7-4629-B10B-4AE61FC27281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDDC9E0B-065C-4CB7-A094-AE5BE0169354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,20 +21,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="5" r:id="rId6"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1099,7 +1086,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1159,36 +1146,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1222,14 +1185,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1244,7 +1203,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1287,7 +1245,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{37148282-7D1D-486F-BE9F-624476633CA1}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{A1704E41-003A-4EC3-B072-B2F8E1648D60}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1317,10 +1275,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99FBAFA2-F9E8-41D8-A5AC-F4445B8B76BF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4138A6C9-1E18-47DA-A664-3985C93592BC}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1358,7 +1316,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5D35EB1-89FC-483C-8205-AE26D8F152E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{182C682E-B827-42C1-B4B6-BA61B14FB22B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1421,7 +1379,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3924810-8DE3-4D12-ACCB-644E2294292C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{748D531A-F5E2-4B84-965A-191E4D9E3D2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1440,7 +1398,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF39C2D9-B3D2-833F-340B-A26960DED5D9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{335476B6-1EDC-DD45-2F0C-FF3F43414A47}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1489,7 +1447,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7761ECEA-96C9-D9DC-1D46-89BC127B88DB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF9E425-0D5C-3A21-2E37-6CDC301D1D6E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1508,7 +1466,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37747C42-2B83-0528-6B17-9250725D5046}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCCE2D60-D528-1C26-4B5B-61BE8FF39288}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1539,7 +1497,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0409334E-0731-A884-CAB6-9555129D83F1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC0D2975-8A8C-BBAD-4109-E94D633B0114}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1570,7 +1528,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8373D4B-17B2-761C-FAA2-5EC8AE287B21}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED44A5FD-7A31-00FF-A269-8E20243961B7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1613,7 +1571,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A43BA4B7-AC35-4662-B67D-E1B1496AC73D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61970EB1-8588-4729-B1E7-15F08308FB2B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1651,7 +1609,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{190C5047-4BFD-4846-A5D0-79452ACC475E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE4ED9E3-7CAA-449A-AEA8-9A440FAA0148}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1694,7 +1652,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8DDA28F-20D1-4C46-8436-35AD9E4A073C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07F98D67-24A6-4143-85C2-C0838E3B2977}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2007,7 +1965,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B53979-D21F-47CD-9299-4BCE4DDBFB3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCBE41C-55F4-4D0A-AE67-70B941CC7128}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2019,98 +1977,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="40"/>
-    <col min="6" max="6" width="2" style="40" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="40" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="40"/>
+    <col min="1" max="5" width="12.5703125" style="37"/>
+    <col min="6" max="6" width="2" style="37" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="37" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="37"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="39"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="39"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="39"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="39"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="39"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="39"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="39"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="39"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="39"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="39"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="39"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="39"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="39"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="39"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="39"/>
+      <c r="F15" s="36"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="39"/>
+      <c r="F16" s="36"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="39"/>
+      <c r="F17" s="36"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="39"/>
+      <c r="F18" s="36"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="39"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="39"/>
+      <c r="F20" s="36"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="39"/>
+      <c r="F21" s="36"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="39"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="39"/>
+      <c r="F23" s="36"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="39"/>
+      <c r="F24" s="36"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="39"/>
+      <c r="F25" s="36"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="39"/>
+      <c r="F26" s="36"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="39"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="39"/>
+      <c r="F28" s="36"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="39"/>
+      <c r="F29" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5257,19 +5215,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>256</v>
       </c>
     </row>
@@ -5292,68 +5250,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="17" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="17" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="17" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="17" t="s">
         <v>260</v>
       </c>
     </row>
@@ -5371,225 +5329,225 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
+    <col min="10" max="10" width="72.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="20" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="14">
         <v>385397</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="21">
         <v>3120</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="21">
         <v>312</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="14">
         <v>15</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="22">
         <v>24869</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="14">
         <v>429252</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="21">
         <v>2550.9</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="21">
         <v>255.09</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="22">
         <v>24885</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="14">
         <v>537409</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="21">
         <v>520</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="21">
         <v>360.1</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="14">
         <v>11</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="22">
         <v>24889</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="14">
         <v>537268</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="21">
         <v>838.2</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="21">
         <v>580.72</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="14">
         <v>21</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="22">
         <v>24878</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="14">
         <v>453048</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="21">
         <v>735</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="21">
         <v>531.13</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="14">
         <v>10</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="22">
         <v>24896</v>
       </c>
     </row>
@@ -5614,99 +5572,100 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>290</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="24" t="s">
         <v>292</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="25" t="s">
         <v>294</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="25" t="s">
         <v>295</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="23" t="s">
         <v>298</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="23" t="s">
         <v>301</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="23" t="s">
         <v>302</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="23" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="14" t="s">
         <v>304</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="26">
         <v>45839</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="27" t="s">
         <v>305</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="28">
         <v>29486</v>
       </c>
-      <c r="G2" s="31">
+      <c r="G2" s="28">
         <v>4153</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="14" t="s">
         <v>306</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="29" t="s">
         <v>307</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="14" t="s">
         <v>306</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="29" t="s">
         <v>307</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="29" t="s">
         <v>307</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="30" t="s">
         <v>308</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="14" t="s">
         <v>306</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="30" t="s">
         <v>308</v>
       </c>
     </row>
@@ -5731,31 +5690,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>310</v>
       </c>
-      <c r="E1" s="35">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="32">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" s="35">
         <v>171</v>
       </c>
-      <c r="F1" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>275</v>
-      </c>
-      <c r="B2" s="38">
-        <v>171</v>
-      </c>
-      <c r="C2" s="36">
+      <c r="C2" s="33">
         <v>1.1308028038619231E-2</v>
       </c>
     </row>

</xml_diff>